<commit_message>
Cambios finales fase 3
</commit_message>
<xml_diff>
--- a/avances_semanales/fase3/entrada1.xlsx
+++ b/avances_semanales/fase3/entrada1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteb\Documents\GitHub\analisis_vibraciones\avances_semanales\fase3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99DA784-C486-49D7-A061-B61751E3621A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C46D21-AEC4-430A-A682-48EF0F950E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1563,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6411D8F9-1C02-43E4-B965-2ED18DE2C766}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3687,7 +3687,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>